<commit_message>
Fix test pass error for MS-ASCAL
</commit_message>
<xml_diff>
--- a/ExchangeActiveSync/Docs/MS-ASCAL/MS-ASCAL_RequirementSpecification.xlsx
+++ b/ExchangeActiveSync/Docs/MS-ASCAL/MS-ASCAL_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91E1354-7EE2-497A-9E29-19C074219F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59655885-2E08-455E-A273-E9F64E5F5AE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8468" uniqueCount="2549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8468" uniqueCount="2550">
   <si>
     <t>Req ID</t>
   </si>
@@ -7904,6 +7904,9 @@
   </si>
   <si>
     <t>[In StartTime] In protocol version 12.0, 12.1, 14.0, 14.1, 16.0, and 16.1, a Sync command response MUST contain one instance of the StartTime element if more than just [DtStamp (section 2.2.2.18) or] AttendeeType (section 2.2.2.6) has changed.</t>
+  </si>
+  <si>
+    <t>MS-ASCAL_R448002</t>
   </si>
 </sst>
 </file>
@@ -15463,8 +15466,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C225" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C242" sqref="C242"/>
+    <sheetView tabSelected="1" topLeftCell="D1129" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1134" sqref="H1134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -38592,7 +38595,7 @@
     </row>
     <row r="931" spans="1:9">
       <c r="A931" s="22" t="s">
-        <v>2467</v>
+        <v>2549</v>
       </c>
       <c r="B931" s="24" t="s">
         <v>976</v>
@@ -43720,7 +43723,7 @@
         <v>15</v>
       </c>
       <c r="H1134" s="22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I1134" s="34"/>
     </row>

</xml_diff>